<commit_message>
update test cases for add customer and project
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRM_Automation_Testing\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C7339-0743-430E-BDBB-D83BACE2DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE099C1-B545-42A7-B269-C63D31B329F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -760,14 +760,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.53125" customWidth="1"/>
+    <col min="2" max="2" width="24.46484375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +778,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -789,7 +789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,7 +800,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -830,23 +830,23 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" customWidth="1"/>
+    <col min="6" max="6" width="13.46484375" customWidth="1"/>
+    <col min="7" max="7" width="11.53125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.46484375" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.46484375" customWidth="1"/>
+    <col min="12" max="12" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -884,7 +884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -922,7 +922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -972,31 +972,31 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.46484375" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="5" max="5" width="11.53125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" customWidth="1"/>
+    <col min="8" max="8" width="22.1328125" customWidth="1"/>
+    <col min="9" max="9" width="16.86328125" customWidth="1"/>
+    <col min="10" max="10" width="15.796875" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" customWidth="1"/>
+    <col min="12" max="12" width="12.46484375" customWidth="1"/>
+    <col min="13" max="13" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -1263,28 +1263,28 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.86328125" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" customWidth="1"/>
+    <col min="4" max="4" width="11.796875" customWidth="1"/>
+    <col min="5" max="5" width="9.46484375" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="7" max="7" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.86328125" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
update test data for projects
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRM_Automation_Testing\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE099C1-B545-42A7-B269-C63D31B329F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FBDA89-5008-40CF-8D9C-7205C8D9C1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="128">
   <si>
     <t>EMAIL</t>
   </si>
@@ -309,9 +309,6 @@
     <t>SEND_PROJECT_FINISHED</t>
   </si>
   <si>
-    <t>htest1</t>
-  </si>
-  <si>
     <t>htest2</t>
   </si>
   <si>
@@ -409,6 +406,12 @@
   </si>
   <si>
     <t xml:space="preserve">[AUTO_HT] project edit </t>
+  </si>
+  <si>
+    <t>UPDATE_PROJECT_NAME</t>
+  </si>
+  <si>
+    <t>htest1, htest12, hatest13</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -469,9 +472,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -760,14 +771,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.53125" customWidth="1"/>
-    <col min="2" max="2" width="24.46484375" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +789,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -789,7 +800,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,7 +811,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -827,31 +838,31 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" customWidth="1"/>
-    <col min="6" max="6" width="13.46484375" customWidth="1"/>
-    <col min="7" max="7" width="11.53125" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="15.46484375" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14.46484375" customWidth="1"/>
-    <col min="12" max="12" width="15.796875" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -884,9 +895,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>65</v>
@@ -922,9 +933,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
@@ -969,34 +980,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776F527C-2B5B-452D-B09B-948A7D4FA5C6}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.46484375" customWidth="1"/>
-    <col min="2" max="2" width="18.796875" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" customWidth="1"/>
-    <col min="5" max="5" width="11.53125" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" customWidth="1"/>
-    <col min="8" max="8" width="22.1328125" customWidth="1"/>
-    <col min="9" max="9" width="16.86328125" customWidth="1"/>
-    <col min="10" max="10" width="15.796875" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" customWidth="1"/>
-    <col min="12" max="12" width="12.46484375" customWidth="1"/>
-    <col min="13" max="13" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -1040,212 +1050,198 @@
         <v>15</v>
       </c>
       <c r="O1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>21</v>
+      <c r="H2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="I3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="C5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="N2" t="s">
-        <v>120</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="J5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="P5" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N3" t="s">
-        <v>121</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4" t="s">
-        <v>122</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1263,28 +1259,28 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
-    <col min="4" max="4" width="11.796875" customWidth="1"/>
-    <col min="5" max="5" width="9.46484375" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" customWidth="1"/>
-    <col min="7" max="7" width="29.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.53125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -1337,9 +1333,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>35</v>
@@ -1366,7 +1362,7 @@
         <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>42</v>
@@ -1390,9 +1386,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>49</v>
@@ -1419,7 +1415,7 @@
         <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
add test case for deleting project
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRM_Automation_Testing\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FBDA89-5008-40CF-8D9C-7205C8D9C1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE181A92-71A5-4CEA-9A2B-17E79844A2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -771,14 +771,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.53125" customWidth="1"/>
+    <col min="2" max="2" width="24.46484375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +789,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -800,7 +800,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -811,7 +811,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -841,23 +841,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" customWidth="1"/>
+    <col min="6" max="6" width="13.46484375" customWidth="1"/>
+    <col min="7" max="7" width="11.53125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.46484375" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.46484375" customWidth="1"/>
+    <col min="12" max="12" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -895,7 +895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -933,7 +933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -983,30 +983,30 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.46484375" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="5" max="5" width="11.53125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" customWidth="1"/>
+    <col min="8" max="8" width="22.1328125" customWidth="1"/>
+    <col min="9" max="9" width="16.86328125" customWidth="1"/>
+    <col min="10" max="10" width="15.796875" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" customWidth="1"/>
+    <col min="12" max="12" width="12.46484375" customWidth="1"/>
+    <col min="13" max="13" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="22.5546875" customWidth="1"/>
+    <col min="16" max="16" width="22.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>124</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>125</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>124</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>125</v>
       </c>
@@ -1259,28 +1259,28 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.86328125" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" customWidth="1"/>
+    <col min="4" max="4" width="11.796875" customWidth="1"/>
+    <col min="5" max="5" width="9.46484375" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="7" max="7" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.86328125" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
add testcase for creating Task with DataProvider support
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRM_Automation_Testing\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE181A92-71A5-4CEA-9A2B-17E79844A2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71D8475-FD1A-4A08-8721-F325C8E67F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
   <si>
     <t>EMAIL</t>
   </si>
@@ -54,9 +54,6 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>TAG</t>
-  </si>
-  <si>
     <t>CITY</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>htest</t>
-  </si>
-  <si>
     <t>Hà Nội</t>
   </si>
   <si>
@@ -90,21 +84,12 @@
     <t>Vietnamese</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>TYPE_CONFIRM</t>
-  </si>
-  <si>
     <t>10-12-2025</t>
   </si>
   <si>
     <t>TASK_NAME</t>
   </si>
   <si>
-    <t>HOURLY_RATE</t>
-  </si>
-  <si>
     <t>START_DATE</t>
   </si>
   <si>
@@ -117,30 +102,12 @@
     <t>REPEAT_EVERY</t>
   </si>
   <si>
-    <t>NUMBER_REPEAT_EVERY_CUSTOM</t>
-  </si>
-  <si>
-    <t>TYPE_REPEAT_EVERY_CUSTOM</t>
-  </si>
-  <si>
     <t>TOTAL_CYCLES</t>
   </si>
   <si>
-    <t>RELATED_TO</t>
-  </si>
-  <si>
-    <t>ASSIGNEE</t>
-  </si>
-  <si>
-    <t>FOLLOWER</t>
-  </si>
-  <si>
     <t>8.00</t>
   </si>
   <si>
-    <t>12-12-2025</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -156,24 +123,12 @@
     <t>6</t>
   </si>
   <si>
-    <t>Admin Anh Tester</t>
-  </si>
-  <si>
     <t>Admin Example</t>
   </si>
   <si>
-    <t>htest switch to frame description</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
-    <t>CHECKED</t>
-  </si>
-  <si>
-    <t>16-12-2025</t>
-  </si>
-  <si>
     <t>14-12-2025</t>
   </si>
   <si>
@@ -186,15 +141,6 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>TEST_TYPE</t>
-  </si>
-  <si>
-    <t>ADD</t>
-  </si>
-  <si>
-    <t>EDIT</t>
-  </si>
-  <si>
     <t>success</t>
   </si>
   <si>
@@ -372,12 +318,6 @@
     <t>Project</t>
   </si>
   <si>
-    <t xml:space="preserve">[AUTO] htest task add </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[AUTO] htest task edit </t>
-  </si>
-  <si>
     <t>VAT_NUMBER</t>
   </si>
   <si>
@@ -412,6 +352,72 @@
   </si>
   <si>
     <t>htest1, htest12, hatest13</t>
+  </si>
+  <si>
+    <t>FOLLOWERS</t>
+  </si>
+  <si>
+    <t>ASSIGNEES</t>
+  </si>
+  <si>
+    <t>MILESTONE</t>
+  </si>
+  <si>
+    <t>PUBLIC</t>
+  </si>
+  <si>
+    <t>BILLABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[AUTO_HT] task add </t>
+  </si>
+  <si>
+    <t>[AUTO_HT] task edit</t>
+  </si>
+  <si>
+    <t>02-02-2026</t>
+  </si>
+  <si>
+    <t>01-02-2026</t>
+  </si>
+  <si>
+    <t>16-02-2026</t>
+  </si>
+  <si>
+    <t>INFINITY</t>
+  </si>
+  <si>
+    <t>htest add task description</t>
+  </si>
+  <si>
+    <t>htest edit task description</t>
+  </si>
+  <si>
+    <t>htest1, htest2</t>
+  </si>
+  <si>
+    <t>htest2, htest3</t>
+  </si>
+  <si>
+    <t>Project Manager, Admin Anh Tester, Admin Example</t>
+  </si>
+  <si>
+    <t>Project Manager, Admin Anh Tester</t>
+  </si>
+  <si>
+    <t>Project Manager, Admin Example</t>
+  </si>
+  <si>
+    <t>RELATED_TO_TYPE</t>
+  </si>
+  <si>
+    <t>REPEAT_INTERVAL_VALUE</t>
+  </si>
+  <si>
+    <t>REPEAT_INTERVAL_UNIT</t>
+  </si>
+  <si>
+    <t>UPDATE_TASK_NAME</t>
   </si>
 </sst>
 </file>
@@ -786,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -797,7 +803,7 @@
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -808,7 +814,7 @@
         <v>123456</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -819,7 +825,7 @@
         <v>1234567</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -859,10 +865,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -871,104 +877,104 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -982,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776F527C-2B5B-452D-B09B-948A7D4FA5C6}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1008,240 +1014,240 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="P2" s="7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="K3" s="8" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="J4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="7" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="K5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="N5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="M5" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="O5" s="8" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1253,190 +1259,197 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C77C47-9B28-4F45-A10C-C7E9B32AD41D}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" customWidth="1"/>
-    <col min="4" max="4" width="11.796875" customWidth="1"/>
-    <col min="5" max="5" width="9.46484375" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" customWidth="1"/>
-    <col min="7" max="7" width="29.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.53125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.86328125" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="K2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="M2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="M3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support multi-file attachment in task flow
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dataCRM.xlsx
+++ b/src/test/resources/testdata/dataCRM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRM_Automation_Testing\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71D8475-FD1A-4A08-8721-F325C8E67F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4A8B01-3756-459A-9DD2-4CBAB8879234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
   <si>
     <t>EMAIL</t>
   </si>
@@ -105,9 +105,6 @@
     <t>TOTAL_CYCLES</t>
   </si>
   <si>
-    <t>8.00</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -418,6 +415,12 @@
   </si>
   <si>
     <t>UPDATE_TASK_NAME</t>
+  </si>
+  <si>
+    <t>ATTACH_FILE</t>
+  </si>
+  <si>
+    <t>MauCT01.doc, HDTT.doc</t>
   </si>
 </sst>
 </file>
@@ -792,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -803,7 +806,7 @@
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -814,7 +817,7 @@
         <v>123456</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -825,7 +828,7 @@
         <v>1234567</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -877,16 +880,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
         <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -903,28 +906,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>15</v>
@@ -933,7 +936,7 @@
         <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
         <v>16</v>
@@ -941,40 +944,40 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>56</v>
       </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s">
         <v>57</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1014,240 +1017,240 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="P3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1259,197 +1262,203 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C77C47-9B28-4F45-A10C-C7E9B32AD41D}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.06640625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>110</v>
+      <c r="D1" t="s">
+        <v>129</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="L1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>108</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="Q1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>129</v>
+      <c r="S1" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="57" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
-        <v>43</v>
+    <row r="2" spans="1:19" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="7" t="s">
+      <c r="M3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="Q3" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>42</v>
+        <v>121</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>